<commit_message>
bugs fix and add new test codes
</commit_message>
<xml_diff>
--- a/SCPI_Commands/CMD_Table_BM2.xlsx
+++ b/SCPI_Commands/CMD_Table_BM2.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Arduino Sketch\sw_2021-11\Git\BatteryCommunicationSCPI\SCPI_Commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36FB72E-7CD3-4CA8-BDA4-77511E56BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F1D09-EC73-4688-B9D6-54CF3DD0B79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{08137141-3C22-45DC-8C5E-B97C4EB4BE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="661" xr2:uid="{08137141-3C22-45DC-8C5E-B97C4EB4BE89}"/>
   </bookViews>
   <sheets>
-    <sheet name="BM2 Telemetry List" sheetId="1" r:id="rId1"/>
-    <sheet name="BM2 TM List sort by CMD" sheetId="6" r:id="rId2"/>
-    <sheet name="Selected TM for DAQ" sheetId="7" r:id="rId3"/>
-    <sheet name="BM2 TM List sort by Length" sheetId="5" r:id="rId4"/>
-    <sheet name="BM2 SCPI Commands" sheetId="4" r:id="rId5"/>
+    <sheet name="BM2 Func Test 27-01-22" sheetId="9" r:id="rId1"/>
+    <sheet name="BM2 Telemetry List" sheetId="1" r:id="rId2"/>
+    <sheet name="BM2 TM List sort by CMD" sheetId="6" r:id="rId3"/>
+    <sheet name="Selected TM for DAQ" sheetId="7" r:id="rId4"/>
+    <sheet name="BM2 TM List sort by Length" sheetId="5" r:id="rId5"/>
+    <sheet name="BM2 SCPI Commands" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="305">
   <si>
     <t>ID</t>
   </si>
@@ -995,12 +994,54 @@
   <si>
     <t>Resets the state of the BQ34Z Gas Gauge chip. Use only when directed.</t>
   </si>
+  <si>
+    <t>[1:11974] 651_2cell_HE4_v9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Requested DATA</t>
+  </si>
+  <si>
+    <t>0xC0,0x00</t>
+  </si>
+  <si>
+    <t>0x00,0x00</t>
+  </si>
+  <si>
+    <t>0x00,0x04</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00,0x00
+</t>
+  </si>
+  <si>
+    <t>0x00,0x00,0x00</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>0x00,0x00,0x00,0x00,0x00,0x00,0x00,0x00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x45,0x80
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1069,8 +1110,15 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1098,6 +1146,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1250,6 +1310,91 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1563,11 +1708,1361 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB8B45-8D73-4944-8685-13D5D1F0E749}">
+  <dimension ref="A1:H55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" style="42" customWidth="1"/>
+    <col min="4" max="4" width="54" style="43" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.109375" style="43" customWidth="1"/>
+    <col min="7" max="7" width="16" style="42" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" style="44" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="64" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="50">
+        <v>12</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="52">
+        <v>0</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="52">
+        <v>45</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="50">
+        <v>9</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="55">
+        <v>8</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="55">
+        <v>15</v>
+      </c>
+      <c r="F3" s="56"/>
+      <c r="G3" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="44">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="50">
+        <v>13</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="55">
+        <v>9</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="55">
+        <v>15</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" s="44">
+        <v>7089</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A5" s="50">
+        <v>14</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="55">
+        <v>10</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="55">
+        <v>15</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="44">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <v>15</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="55">
+        <v>11</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="55">
+        <v>15</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="H6" s="44">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="50">
+        <v>16</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="58">
+        <v>13</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="58">
+        <v>14</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="44">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <v>17</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="58">
+        <v>14</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="58">
+        <v>14</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="44">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <v>18</v>
+      </c>
+      <c r="B9" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="58">
+        <v>15</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="58">
+        <v>15</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="44">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50">
+        <v>19</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="58">
+        <v>16</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="58">
+        <v>15</v>
+      </c>
+      <c r="F10" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="44">
+        <v>6686</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <v>20</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="58">
+        <v>17</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="58">
+        <v>15</v>
+      </c>
+      <c r="F11" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="44">
+        <v>2397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="50">
+        <v>21</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="55">
+        <v>18</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="55">
+        <v>15</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="44">
+        <v>2395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="50">
+        <v>22</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="55">
+        <v>19</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="55">
+        <v>15</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" s="44">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <v>23</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="55">
+        <v>20</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="55">
+        <v>15</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="44">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="50">
+        <v>24</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="55">
+        <v>21</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="55">
+        <v>15</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="H15" s="44">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="50">
+        <v>25</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="58">
+        <v>22</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="58">
+        <v>15</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>26</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="55">
+        <v>23</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="55">
+        <v>15</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="50">
+        <v>27</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="58">
+        <v>24</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="58">
+        <v>15</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="44">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>28</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="58">
+        <v>25</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="58">
+        <v>15</v>
+      </c>
+      <c r="F19" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="44">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="50">
+        <v>29</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="58">
+        <v>28</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="58">
+        <v>17</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="50">
+        <v>30</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="58">
+        <v>29</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="58">
+        <v>17</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="50">
+        <v>31</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="58">
+        <v>30</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="58">
+        <v>17</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="50">
+        <v>32</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="58">
+        <v>31</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="58">
+        <v>17</v>
+      </c>
+      <c r="F23" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="50">
+        <v>33</v>
+      </c>
+      <c r="B24" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="58">
+        <v>32</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="58">
+        <v>17</v>
+      </c>
+      <c r="F24" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="50">
+        <v>34</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="55">
+        <v>33</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="55">
+        <v>15</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="44">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="50">
+        <v>35</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="55">
+        <v>34</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="55">
+        <v>15</v>
+      </c>
+      <c r="F26" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="H26" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="50">
+        <v>36</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="60">
+        <v>36</v>
+      </c>
+      <c r="D27" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="55">
+        <v>14</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="H27" s="44">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="50">
+        <v>37</v>
+      </c>
+      <c r="B28" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="58">
+        <v>37</v>
+      </c>
+      <c r="D28" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="58">
+        <v>15</v>
+      </c>
+      <c r="F28" s="59" t="s">
+        <v>143</v>
+      </c>
+      <c r="H28" s="44">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="50">
+        <v>38</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="58">
+        <v>38</v>
+      </c>
+      <c r="D29" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="58">
+        <v>15</v>
+      </c>
+      <c r="F29" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="44">
+        <v>7328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="50">
+        <v>1</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="55">
+        <v>48</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="55">
+        <v>15</v>
+      </c>
+      <c r="F30" s="56"/>
+      <c r="G30" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30" s="44">
+        <v>2945</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="50">
+        <v>2</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="55">
+        <v>49</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="55">
+        <v>15</v>
+      </c>
+      <c r="F31" s="56"/>
+      <c r="G31" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="H31" s="44">
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="50">
+        <v>3</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="55">
+        <v>50</v>
+      </c>
+      <c r="D32" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="55">
+        <v>15</v>
+      </c>
+      <c r="F32" s="56"/>
+      <c r="G32" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="H32" s="44">
+        <v>2955</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="50">
+        <v>4</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="55">
+        <v>51</v>
+      </c>
+      <c r="D33" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="55">
+        <v>15</v>
+      </c>
+      <c r="F33" s="56"/>
+      <c r="G33" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="H33" s="44">
+        <v>2951</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="50">
+        <v>39</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="58">
+        <v>52</v>
+      </c>
+      <c r="D34" s="59" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="58">
+        <v>14</v>
+      </c>
+      <c r="F34" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="H34" s="44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="50">
+        <v>40</v>
+      </c>
+      <c r="B35" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="58">
+        <v>53</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="58">
+        <v>28</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="71" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="67">
+        <v>41</v>
+      </c>
+      <c r="B36" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="69">
+        <v>54</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="69">
+        <v>17</v>
+      </c>
+      <c r="F36" s="70"/>
+      <c r="H36" s="72" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="50">
+        <v>42</v>
+      </c>
+      <c r="B37" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="58">
+        <v>55</v>
+      </c>
+      <c r="D37" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="58">
+        <v>45</v>
+      </c>
+      <c r="F37" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" s="66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="50">
+        <v>43</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="58">
+        <v>56</v>
+      </c>
+      <c r="D38" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="58">
+        <v>45</v>
+      </c>
+      <c r="F38" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="50">
+        <v>44</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="58">
+        <v>57</v>
+      </c>
+      <c r="D39" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="58">
+        <v>15</v>
+      </c>
+      <c r="F39" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="H39" s="66" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="50">
+        <v>45</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="58">
+        <v>58</v>
+      </c>
+      <c r="D40" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="58">
+        <v>21</v>
+      </c>
+      <c r="F40" s="59"/>
+      <c r="H40" s="44" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="50">
+        <v>46</v>
+      </c>
+      <c r="B41" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="55">
+        <v>60</v>
+      </c>
+      <c r="D41" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="55">
+        <v>15</v>
+      </c>
+      <c r="F41" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="50">
+        <v>47</v>
+      </c>
+      <c r="B42" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="55">
+        <v>61</v>
+      </c>
+      <c r="D42" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" s="55">
+        <v>15</v>
+      </c>
+      <c r="F42" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="H42" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="50">
+        <v>48</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="55">
+        <v>62</v>
+      </c>
+      <c r="D43" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="55">
+        <v>15</v>
+      </c>
+      <c r="F43" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="H43" s="44">
+        <v>3564</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="50">
+        <v>49</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="55">
+        <v>63</v>
+      </c>
+      <c r="D44" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="55">
+        <v>15</v>
+      </c>
+      <c r="F44" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="44">
+        <v>3523</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="50">
+        <v>5</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="55">
+        <v>71</v>
+      </c>
+      <c r="D45" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="55">
+        <v>15</v>
+      </c>
+      <c r="F45" s="56"/>
+      <c r="G45" s="42" t="s">
+        <v>227</v>
+      </c>
+      <c r="H45" s="44">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="50">
+        <v>6</v>
+      </c>
+      <c r="B46" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="55">
+        <v>72</v>
+      </c>
+      <c r="D46" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="55">
+        <v>15</v>
+      </c>
+      <c r="F46" s="56"/>
+      <c r="G46" s="63" t="s">
+        <v>228</v>
+      </c>
+      <c r="H46" s="44">
+        <v>2952</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="50">
+        <v>7</v>
+      </c>
+      <c r="B47" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="55">
+        <v>73</v>
+      </c>
+      <c r="D47" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="55">
+        <v>15</v>
+      </c>
+      <c r="F47" s="56"/>
+      <c r="G47" s="63" t="s">
+        <v>229</v>
+      </c>
+      <c r="H47" s="44">
+        <v>2951</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="50">
+        <v>8</v>
+      </c>
+      <c r="B48" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="55">
+        <v>74</v>
+      </c>
+      <c r="D48" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="55">
+        <v>15</v>
+      </c>
+      <c r="F48" s="56"/>
+      <c r="G48" s="63" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" s="44">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="78" x14ac:dyDescent="0.3">
+      <c r="A49" s="50">
+        <v>50</v>
+      </c>
+      <c r="B49" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="55">
+        <v>77</v>
+      </c>
+      <c r="D49" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="55">
+        <v>14</v>
+      </c>
+      <c r="F49" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="G49" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="H49" s="44" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="50">
+        <v>51</v>
+      </c>
+      <c r="B50" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="58">
+        <v>78</v>
+      </c>
+      <c r="D50" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50" s="58">
+        <v>46</v>
+      </c>
+      <c r="F50" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="H50" s="44" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="50">
+        <v>52</v>
+      </c>
+      <c r="B51" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="62">
+        <v>84</v>
+      </c>
+      <c r="D51" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="58">
+        <v>15</v>
+      </c>
+      <c r="F51" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="H51" s="66" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="50">
+        <v>53</v>
+      </c>
+      <c r="B52" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="55">
+        <v>90</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="55">
+        <v>15</v>
+      </c>
+      <c r="F52" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="G52" s="42" t="s">
+        <v>232</v>
+      </c>
+      <c r="H52" s="44">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="50">
+        <v>54</v>
+      </c>
+      <c r="B53" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="60">
+        <v>93</v>
+      </c>
+      <c r="D53" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="55">
+        <v>15</v>
+      </c>
+      <c r="F53" s="56"/>
+      <c r="G53" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="H53" s="44">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="50">
+        <v>11</v>
+      </c>
+      <c r="B54" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="52">
+        <v>114</v>
+      </c>
+      <c r="D54" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="52">
+        <v>15</v>
+      </c>
+      <c r="F54" s="53"/>
+      <c r="H54" s="44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="50">
+        <v>10</v>
+      </c>
+      <c r="B55" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="55">
+        <v>115</v>
+      </c>
+      <c r="D55" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="55">
+        <v>15</v>
+      </c>
+      <c r="F55" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="H55" s="44">
+        <v>2817</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D615A0E6-39B9-4511-9BEC-49C2F5170D32}">
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2660,12 +4155,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43960A8-2D45-492F-8807-592CE1DF8A63}">
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3843,15 +5338,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038C5D07-134F-48D3-B9ED-66BB92A75427}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4492,11 +5987,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B352FE6-8A99-4C33-BCE2-CE73CD7C4F2A}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B42" sqref="B42:F42"/>
     </sheetView>
   </sheetViews>
@@ -5026,7 +6521,7 @@
       </c>
       <c r="F26" s="36"/>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>2</v>
       </c>
@@ -5044,7 +6539,7 @@
       </c>
       <c r="F27" s="36"/>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="39">
         <v>3</v>
       </c>
@@ -5062,7 +6557,7 @@
       </c>
       <c r="F28" s="36"/>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A29" s="39">
         <v>4</v>
       </c>
@@ -5593,7 +7088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C969AE5-BCDE-408B-A586-77627CC4BF76}">
   <dimension ref="A1:S13"/>
   <sheetViews>

</xml_diff>

<commit_message>
minor update and bug fix
</commit_message>
<xml_diff>
--- a/SCPI_Commands/CMD_Table_BM2.xlsx
+++ b/SCPI_Commands/CMD_Table_BM2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Arduino Sketch\sw_2021-11\Git\BatteryCommunicationSCPI\SCPI_Commands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F1D09-EC73-4688-B9D6-54CF3DD0B79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B28483-7019-4860-8F41-8CD069B46D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="661" xr2:uid="{08137141-3C22-45DC-8C5E-B97C4EB4BE89}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="661" xr2:uid="{08137141-3C22-45DC-8C5E-B97C4EB4BE89}"/>
   </bookViews>
   <sheets>
     <sheet name="BM2 Func Test 27-01-22" sheetId="9" r:id="rId1"/>
@@ -1053,38 +1053,45 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1098,17 +1105,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1711,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB8B45-8D73-4944-8685-13D5D1F0E749}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1880,19 +1889,19 @@
       <c r="A7" s="50">
         <v>16</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="58">
+      <c r="C7" s="55">
         <v>13</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="58">
+      <c r="E7" s="55">
         <v>14</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="56" t="s">
         <v>59</v>
       </c>
       <c r="H7" s="44">
@@ -1903,19 +1912,19 @@
       <c r="A8" s="50">
         <v>17</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="58">
+      <c r="C8" s="55">
         <v>14</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="58">
+      <c r="E8" s="55">
         <v>14</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="56" t="s">
         <v>63</v>
       </c>
       <c r="H8" s="44">
@@ -1926,19 +1935,19 @@
       <c r="A9" s="50">
         <v>18</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="58">
-        <v>15</v>
-      </c>
-      <c r="D9" s="59" t="s">
+      <c r="C9" s="55">
+        <v>15</v>
+      </c>
+      <c r="D9" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="58">
-        <v>15</v>
-      </c>
-      <c r="F9" s="59" t="s">
+      <c r="E9" s="55">
+        <v>15</v>
+      </c>
+      <c r="F9" s="56" t="s">
         <v>67</v>
       </c>
       <c r="H9" s="44">
@@ -1972,19 +1981,19 @@
       <c r="A11" s="50">
         <v>20</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="55">
         <v>17</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="58">
-        <v>15</v>
-      </c>
-      <c r="F11" s="59" t="s">
+      <c r="E11" s="55">
+        <v>15</v>
+      </c>
+      <c r="F11" s="56" t="s">
         <v>75</v>
       </c>
       <c r="H11" s="44">
@@ -3515,7 +3524,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="39">
         <v>23</v>
       </c>
@@ -3615,7 +3624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="39">
         <v>28</v>
       </c>
@@ -4809,7 +4818,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>2</v>
       </c>
@@ -4830,7 +4839,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="39">
         <v>3</v>
       </c>
@@ -4851,7 +4860,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="39">
         <v>4</v>
       </c>
@@ -6521,7 +6530,7 @@
       </c>
       <c r="F26" s="36"/>
     </row>
-    <row r="27" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>2</v>
       </c>
@@ -6539,7 +6548,7 @@
       </c>
       <c r="F27" s="36"/>
     </row>
-    <row r="28" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="39">
         <v>3</v>
       </c>
@@ -6557,7 +6566,7 @@
       </c>
       <c r="F28" s="36"/>
     </row>
-    <row r="29" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39">
         <v>4</v>
       </c>

</xml_diff>